<commit_message>
commit sleep schedule code
</commit_message>
<xml_diff>
--- a/touchGFX/Application/assets/texts/texts.xlsx
+++ b/touchGFX/Application/assets/texts/texts.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\L2200_TouchGFX\L2200_new\touchGFX\Application\assets\texts\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8196" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Typography" sheetId="1" r:id="rId1"/>
@@ -20,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="341" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="185">
   <si>
     <t>Font</t>
   </si>
@@ -284,37 +279,6 @@
   </si>
   <si>
     <t>Datepicker_Day_28</t>
-  </si>
-  <si>
-    <t>1
-2
-3
-4
-5
-6
-7
-8
-9
-10
-11
-12
-13
-14
-15
-16
-17
-18
-19
-20
-21
-22
-23
-24
-25
-26
-27
-28</t>
-    <phoneticPr fontId="8" type="noConversion"/>
   </si>
   <si>
     <t>Datepicker_Day_29</t>
@@ -770,6 +734,58 @@
   </si>
   <si>
     <t>!”"#*%&amp;()'$+-@_, .:;?/~±×÷•º`´{}©£€^®¥_=[]¡¢|\¿&gt;&lt;</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>time_picker_duration</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sleepduration</t>
+  </si>
+  <si>
+    <t>Sleepduration</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>1
+2
+3
+4
+5
+6
+7
+8
+9
+10
+11
+12
+13
+14
+15
+16
+17
+18
+19
+20
+21
+22
+23
+24
+25
+26
+27
+28</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>15 sec
+30 sec
+1 min
+2 min
+5 min
+15 min
+30 min</t>
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
 </sst>
@@ -1128,7 +1144,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1168,8 +1184,14 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="81" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="81" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="82">
@@ -1951,29 +1973,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:O22"/>
+  <dimension ref="B1:O23"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+    <sheetView showGridLines="0" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="0.28515625" customWidth="1"/>
-    <col min="2" max="2" width="25.7109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="26.85546875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="10.42578125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="0.33203125" customWidth="1"/>
+    <col min="2" max="2" width="25.6640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="26.88671875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="10.44140625" style="1" customWidth="1"/>
     <col min="5" max="5" width="10" style="1" customWidth="1"/>
-    <col min="6" max="6" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="51.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.140625" customWidth="1"/>
-    <col min="10" max="10" width="4.5703125" customWidth="1"/>
-    <col min="11" max="11" width="20.140625" customWidth="1"/>
-    <col min="12" max="12" width="84.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="51.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.109375" customWidth="1"/>
+    <col min="10" max="10" width="4.5546875" customWidth="1"/>
+    <col min="11" max="11" width="20.109375" customWidth="1"/>
+    <col min="12" max="12" width="84.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.33203125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="11" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="19.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:15" ht="129" hidden="1" customHeight="1">
@@ -1982,19 +2004,19 @@
       <c r="D1"/>
       <c r="E1"/>
     </row>
-    <row r="2" spans="2:15" ht="39.950000000000003" customHeight="1" thickBot="1">
-      <c r="B2" s="27" t="s">
+    <row r="2" spans="2:15" ht="39.9" customHeight="1" thickBot="1">
+      <c r="B2" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
-      <c r="E2" s="27"/>
-      <c r="F2" s="27"/>
-      <c r="G2" s="27"/>
-      <c r="H2" s="27"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="28"/>
+      <c r="F2" s="28"/>
+      <c r="G2" s="28"/>
+      <c r="H2" s="28"/>
       <c r="I2" s="3"/>
     </row>
-    <row r="3" spans="2:15" ht="15.75" thickBot="1">
+    <row r="3" spans="2:15" ht="15" thickBot="1">
       <c r="B3" s="17" t="s">
         <v>8</v>
       </c>
@@ -2022,7 +2044,7 @@
     </row>
     <row r="4" spans="2:15">
       <c r="B4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C4" t="s">
         <v>40</v>
@@ -2078,7 +2100,7 @@
     </row>
     <row r="6" spans="2:15">
       <c r="B6" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C6" t="s">
         <v>40</v>
@@ -2117,10 +2139,10 @@
         <v>1</v>
       </c>
       <c r="G7" t="s">
+        <v>90</v>
+      </c>
+      <c r="H7" t="s">
         <v>91</v>
-      </c>
-      <c r="H7" t="s">
-        <v>92</v>
       </c>
       <c r="K7" s="7" t="s">
         <v>15</v>
@@ -2223,7 +2245,7 @@
     </row>
     <row r="11" spans="2:15">
       <c r="B11" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C11" t="s">
         <v>40</v>
@@ -2235,16 +2257,16 @@
         <v>1</v>
       </c>
       <c r="G11" t="s">
+        <v>92</v>
+      </c>
+      <c r="H11" t="s">
         <v>93</v>
-      </c>
-      <c r="H11" t="s">
-        <v>94</v>
       </c>
       <c r="K11" s="15"/>
     </row>
     <row r="12" spans="2:15">
       <c r="B12" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C12" t="s">
         <v>40</v>
@@ -2256,10 +2278,10 @@
         <v>1</v>
       </c>
       <c r="G12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H12" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="L12" s="16" t="s">
         <v>35</v>
@@ -2267,7 +2289,7 @@
     </row>
     <row r="13" spans="2:15">
       <c r="B13" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C13" t="s">
         <v>40</v>
@@ -2281,10 +2303,10 @@
     </row>
     <row r="14" spans="2:15">
       <c r="B14" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C14" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D14">
         <v>75</v>
@@ -2295,7 +2317,7 @@
     </row>
     <row r="15" spans="2:15">
       <c r="B15" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C15" t="s">
         <v>40</v>
@@ -2307,12 +2329,12 @@
         <v>1</v>
       </c>
       <c r="H15" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="16" spans="2:15">
       <c r="B16" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C16" t="s">
         <v>40</v>
@@ -2327,12 +2349,12 @@
         <v>25</v>
       </c>
       <c r="G16" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="17" spans="2:8">
       <c r="B17" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C17" t="s">
         <v>40</v>
@@ -2346,7 +2368,7 @@
     </row>
     <row r="18" spans="2:8">
       <c r="B18" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C18" t="s">
         <v>40</v>
@@ -2360,7 +2382,7 @@
     </row>
     <row r="19" spans="2:8">
       <c r="B19" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C19" t="s">
         <v>40</v>
@@ -2377,10 +2399,10 @@
     </row>
     <row r="20" spans="2:8">
       <c r="B20" s="22" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C20" s="24" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D20" s="22">
         <v>28</v>
@@ -2392,18 +2414,18 @@
         <v>25</v>
       </c>
       <c r="G20" s="25" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="H20" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="21" spans="2:8">
       <c r="B21" s="22" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C21" s="24" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D21" s="22">
         <v>20</v>
@@ -2415,23 +2437,37 @@
         <v>25</v>
       </c>
       <c r="G21" s="26" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="H21" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="22" spans="2:8">
       <c r="B22" s="22" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C22" s="24" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D22" s="22">
         <v>24</v>
       </c>
       <c r="E22" s="22">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="2:8">
+      <c r="B23" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="C23" s="24" t="s">
+        <v>176</v>
+      </c>
+      <c r="D23" s="22">
+        <v>16</v>
+      </c>
+      <c r="E23" s="22">
         <v>4</v>
       </c>
     </row>
@@ -2453,21 +2489,21 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:J63"/>
+  <dimension ref="B1:J64"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A44" workbookViewId="0">
-      <selection activeCell="F58" sqref="F58"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A56" workbookViewId="0">
+      <selection activeCell="E64" sqref="E64"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="0.28515625" customWidth="1"/>
-    <col min="2" max="2" width="54.7109375" style="1" customWidth="1"/>
-    <col min="3" max="4" width="25.7109375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="35.7109375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="50.7109375" style="1" customWidth="1"/>
-    <col min="7" max="8" width="8.7109375" style="1" customWidth="1"/>
-    <col min="9" max="9" width="54.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="0.33203125" customWidth="1"/>
+    <col min="2" max="2" width="54.6640625" style="1" customWidth="1"/>
+    <col min="3" max="4" width="25.6640625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="35.6640625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="50.6640625" style="1" customWidth="1"/>
+    <col min="7" max="8" width="8.6640625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="54.33203125" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:10" ht="129" hidden="1" customHeight="1">
@@ -2480,17 +2516,17 @@
       <c r="H1"/>
       <c r="I1"/>
     </row>
-    <row r="2" spans="2:10" ht="39.950000000000003" customHeight="1">
-      <c r="B2" s="27" t="s">
+    <row r="2" spans="2:10" ht="39.9" customHeight="1">
+      <c r="B2" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
-      <c r="E2" s="27"/>
-      <c r="F2" s="27"/>
-      <c r="G2" s="27"/>
-      <c r="H2" s="27"/>
-      <c r="I2" s="27"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="28"/>
+      <c r="F2" s="28"/>
+      <c r="G2" s="28"/>
+      <c r="H2" s="28"/>
+      <c r="I2" s="28"/>
       <c r="J2" t="s">
         <v>13</v>
       </c>
@@ -2529,7 +2565,7 @@
         <v>57</v>
       </c>
       <c r="D4" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E4" t="s">
         <v>43</v>
@@ -2731,7 +2767,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="19" spans="2:5">
+    <row r="19" spans="2:5" ht="409.6">
       <c r="B19" t="s">
         <v>72</v>
       </c>
@@ -2741,13 +2777,13 @@
       <c r="D19" t="s">
         <v>42</v>
       </c>
-      <c r="E19" t="s">
-        <v>73</v>
+      <c r="E19" s="29" t="s">
+        <v>183</v>
       </c>
     </row>
     <row r="20" spans="2:5">
       <c r="B20" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C20" t="s">
         <v>68</v>
@@ -2756,12 +2792,12 @@
         <v>42</v>
       </c>
       <c r="E20" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="21" spans="2:5">
       <c r="B21" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C21" t="s">
         <v>68</v>
@@ -2770,12 +2806,12 @@
         <v>42</v>
       </c>
       <c r="E21" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="22" spans="2:5">
       <c r="B22" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C22" t="s">
         <v>68</v>
@@ -2784,43 +2820,43 @@
         <v>42</v>
       </c>
       <c r="E22" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="23" spans="2:5">
       <c r="B23" t="s">
+        <v>79</v>
+      </c>
+      <c r="C23" t="s">
         <v>80</v>
       </c>
-      <c r="C23" t="s">
+      <c r="D23" t="s">
+        <v>42</v>
+      </c>
+      <c r="E23" t="s">
         <v>81</v>
-      </c>
-      <c r="D23" t="s">
-        <v>42</v>
-      </c>
-      <c r="E23" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="24" spans="2:5">
       <c r="B24" t="s">
+        <v>82</v>
+      </c>
+      <c r="C24" t="s">
+        <v>80</v>
+      </c>
+      <c r="D24" t="s">
+        <v>42</v>
+      </c>
+      <c r="E24" t="s">
         <v>83</v>
-      </c>
-      <c r="C24" t="s">
-        <v>81</v>
-      </c>
-      <c r="D24" t="s">
-        <v>42</v>
-      </c>
-      <c r="E24" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="25" spans="2:5">
       <c r="B25" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C25" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D25" t="s">
         <v>66</v>
@@ -2831,21 +2867,21 @@
     </row>
     <row r="26" spans="2:5">
       <c r="B26" t="s">
+        <v>85</v>
+      </c>
+      <c r="C26" t="s">
+        <v>152</v>
+      </c>
+      <c r="D26" t="s">
+        <v>42</v>
+      </c>
+      <c r="E26" t="s">
         <v>86</v>
-      </c>
-      <c r="C26" t="s">
-        <v>153</v>
-      </c>
-      <c r="D26" t="s">
-        <v>42</v>
-      </c>
-      <c r="E26" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="27" spans="2:5">
       <c r="B27" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C27" t="s">
         <v>57</v>
@@ -2859,24 +2895,24 @@
     </row>
     <row r="28" spans="2:5">
       <c r="B28" t="s">
+        <v>88</v>
+      </c>
+      <c r="C28" t="s">
+        <v>152</v>
+      </c>
+      <c r="D28" t="s">
+        <v>42</v>
+      </c>
+      <c r="E28" t="s">
         <v>89</v>
-      </c>
-      <c r="C28" t="s">
-        <v>153</v>
-      </c>
-      <c r="D28" t="s">
-        <v>42</v>
-      </c>
-      <c r="E28" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="29" spans="2:5">
       <c r="B29" t="s">
+        <v>97</v>
+      </c>
+      <c r="C29" t="s">
         <v>98</v>
-      </c>
-      <c r="C29" t="s">
-        <v>99</v>
       </c>
       <c r="D29" t="s">
         <v>66</v>
@@ -2887,276 +2923,276 @@
     </row>
     <row r="30" spans="2:5">
       <c r="B30" t="s">
+        <v>101</v>
+      </c>
+      <c r="C30" t="s">
+        <v>139</v>
+      </c>
+      <c r="D30" t="s">
+        <v>42</v>
+      </c>
+      <c r="E30" t="s">
         <v>102</v>
-      </c>
-      <c r="C30" t="s">
-        <v>140</v>
-      </c>
-      <c r="D30" t="s">
-        <v>42</v>
-      </c>
-      <c r="E30" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="31" spans="2:5">
       <c r="B31" t="s">
+        <v>103</v>
+      </c>
+      <c r="C31" t="s">
+        <v>139</v>
+      </c>
+      <c r="D31" t="s">
+        <v>42</v>
+      </c>
+      <c r="E31" t="s">
         <v>104</v>
-      </c>
-      <c r="C31" t="s">
-        <v>140</v>
-      </c>
-      <c r="D31" t="s">
-        <v>42</v>
-      </c>
-      <c r="E31" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="32" spans="2:5">
       <c r="B32" t="s">
+        <v>105</v>
+      </c>
+      <c r="C32" t="s">
+        <v>139</v>
+      </c>
+      <c r="D32" t="s">
+        <v>42</v>
+      </c>
+      <c r="E32" t="s">
         <v>106</v>
-      </c>
-      <c r="C32" t="s">
-        <v>140</v>
-      </c>
-      <c r="D32" t="s">
-        <v>42</v>
-      </c>
-      <c r="E32" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="33" spans="2:5">
       <c r="B33" t="s">
+        <v>107</v>
+      </c>
+      <c r="C33" t="s">
+        <v>139</v>
+      </c>
+      <c r="D33" t="s">
+        <v>42</v>
+      </c>
+      <c r="E33" t="s">
         <v>108</v>
-      </c>
-      <c r="C33" t="s">
-        <v>140</v>
-      </c>
-      <c r="D33" t="s">
-        <v>42</v>
-      </c>
-      <c r="E33" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="34" spans="2:5">
       <c r="B34" t="s">
+        <v>109</v>
+      </c>
+      <c r="C34" t="s">
+        <v>139</v>
+      </c>
+      <c r="D34" t="s">
+        <v>42</v>
+      </c>
+      <c r="E34" t="s">
         <v>110</v>
-      </c>
-      <c r="C34" t="s">
-        <v>140</v>
-      </c>
-      <c r="D34" t="s">
-        <v>42</v>
-      </c>
-      <c r="E34" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="35" spans="2:5">
       <c r="B35" t="s">
+        <v>111</v>
+      </c>
+      <c r="C35" t="s">
+        <v>139</v>
+      </c>
+      <c r="D35" t="s">
+        <v>42</v>
+      </c>
+      <c r="E35" t="s">
         <v>112</v>
-      </c>
-      <c r="C35" t="s">
-        <v>140</v>
-      </c>
-      <c r="D35" t="s">
-        <v>42</v>
-      </c>
-      <c r="E35" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="36" spans="2:5">
       <c r="B36" t="s">
+        <v>113</v>
+      </c>
+      <c r="C36" t="s">
+        <v>139</v>
+      </c>
+      <c r="D36" t="s">
+        <v>42</v>
+      </c>
+      <c r="E36" t="s">
         <v>114</v>
-      </c>
-      <c r="C36" t="s">
-        <v>140</v>
-      </c>
-      <c r="D36" t="s">
-        <v>42</v>
-      </c>
-      <c r="E36" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="37" spans="2:5">
       <c r="B37" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C37" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D37" t="s">
         <v>42</v>
       </c>
       <c r="E37" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="38" spans="2:5">
       <c r="B38" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C38" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D38" t="s">
         <v>42</v>
       </c>
       <c r="E38" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="39" spans="2:5">
       <c r="B39" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C39" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D39" t="s">
         <v>42</v>
       </c>
       <c r="E39" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="40" spans="2:5">
       <c r="B40" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C40" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D40" t="s">
         <v>42</v>
       </c>
       <c r="E40" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="41" spans="2:5">
       <c r="B41" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C41" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D41" t="s">
         <v>42</v>
       </c>
       <c r="E41" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="42" spans="2:5">
       <c r="B42" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C42" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D42" t="s">
         <v>42</v>
       </c>
       <c r="E42" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="43" spans="2:5">
       <c r="B43" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C43" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D43" t="s">
         <v>42</v>
       </c>
       <c r="E43" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="44" spans="2:5">
       <c r="B44" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C44" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D44" t="s">
         <v>42</v>
       </c>
       <c r="E44" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="45" spans="2:5">
       <c r="B45" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C45" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D45" t="s">
         <v>42</v>
       </c>
       <c r="E45" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="46" spans="2:5">
       <c r="B46" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C46" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D46" t="s">
         <v>42</v>
       </c>
       <c r="E46" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="47" spans="2:5">
       <c r="B47" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C47" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D47" t="s">
         <v>42</v>
       </c>
       <c r="E47" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="48" spans="2:5">
       <c r="B48" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C48" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D48" t="s">
         <v>42</v>
       </c>
       <c r="E48" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="49" spans="2:5">
       <c r="B49" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C49" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D49" t="s">
         <v>42</v>
@@ -3167,10 +3203,10 @@
     </row>
     <row r="50" spans="2:5">
       <c r="B50" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C50" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D50" t="s">
         <v>66</v>
@@ -3181,10 +3217,10 @@
     </row>
     <row r="51" spans="2:5">
       <c r="B51" t="s">
+        <v>143</v>
+      </c>
+      <c r="C51" t="s">
         <v>144</v>
-      </c>
-      <c r="C51" t="s">
-        <v>145</v>
       </c>
       <c r="D51" t="s">
         <v>66</v>
@@ -3195,170 +3231,184 @@
     </row>
     <row r="52" spans="2:5">
       <c r="B52" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C52" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D52" t="s">
         <v>66</v>
       </c>
       <c r="E52" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="53" spans="2:5">
       <c r="B53" t="s">
+        <v>146</v>
+      </c>
+      <c r="C53" t="s">
+        <v>149</v>
+      </c>
+      <c r="D53" t="s">
+        <v>148</v>
+      </c>
+      <c r="E53" t="s">
         <v>147</v>
-      </c>
-      <c r="C53" t="s">
-        <v>150</v>
-      </c>
-      <c r="D53" t="s">
-        <v>149</v>
-      </c>
-      <c r="E53" t="s">
-        <v>148</v>
       </c>
     </row>
     <row r="54" spans="2:5">
       <c r="B54" t="s">
+        <v>151</v>
+      </c>
+      <c r="C54" t="s">
         <v>152</v>
       </c>
-      <c r="C54" t="s">
-        <v>153</v>
-      </c>
       <c r="D54" t="s">
         <v>42</v>
       </c>
       <c r="E54" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="55" spans="2:5">
       <c r="B55" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C55" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D55" t="s">
         <v>42</v>
       </c>
       <c r="E55" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="56" spans="2:5">
       <c r="B56" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C56" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D56" t="s">
         <v>66</v>
       </c>
       <c r="E56" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="57" spans="2:5">
       <c r="B57" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C57" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D57" t="s">
         <v>42</v>
       </c>
       <c r="E57" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="58" spans="2:5">
       <c r="B58" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C58" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D58" t="s">
         <v>42</v>
       </c>
       <c r="E58" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="59" spans="2:5">
       <c r="B59" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C59" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D59" t="s">
         <v>66</v>
       </c>
       <c r="E59" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="60" spans="2:5">
       <c r="B60" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C60" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D60" t="s">
         <v>66</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="61" spans="2:5">
       <c r="B61" s="22" t="s">
+        <v>168</v>
+      </c>
+      <c r="C61" s="22" t="s">
         <v>169</v>
       </c>
-      <c r="C61" s="22" t="s">
+      <c r="D61" s="22" t="s">
+        <v>42</v>
+      </c>
+      <c r="E61" s="23" t="s">
         <v>170</v>
-      </c>
-      <c r="D61" s="22" t="s">
-        <v>42</v>
-      </c>
-      <c r="E61" s="23" t="s">
-        <v>171</v>
       </c>
     </row>
     <row r="62" spans="2:5">
       <c r="B62" s="22" t="s">
+        <v>171</v>
+      </c>
+      <c r="C62" s="22" t="s">
         <v>172</v>
-      </c>
-      <c r="C62" s="22" t="s">
-        <v>173</v>
       </c>
       <c r="D62" s="22" t="s">
         <v>66</v>
       </c>
       <c r="E62" s="23" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="63" spans="2:5">
       <c r="B63" s="22" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C63" s="22" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D63" s="22" t="s">
         <v>66</v>
       </c>
       <c r="E63" s="23" t="s">
-        <v>176</v>
+        <v>175</v>
+      </c>
+    </row>
+    <row r="64" spans="2:5" ht="187.2">
+      <c r="B64" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="C64" t="s">
+        <v>182</v>
+      </c>
+      <c r="D64" s="22" t="s">
+        <v>42</v>
+      </c>
+      <c r="E64" s="27" t="s">
+        <v>184</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add modal screen for input password
</commit_message>
<xml_diff>
--- a/touchGFX/Application/assets/texts/texts.xlsx
+++ b/touchGFX/Application/assets/texts/texts.xlsx
@@ -1,21 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\L2200_TouchGFX\L2200_new\touchGFX\Application\assets\texts\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8196" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Typography" sheetId="1" r:id="rId1"/>
     <sheet name="Translation" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="145621" calcMode="manual" fullPrecision="0"/>
+  <calcPr calcId="145621" fullPrecision="0" calcOnSave="0" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="209">
   <si>
     <t>Font</t>
   </si>
@@ -279,6 +284,37 @@
   </si>
   <si>
     <t>Datepicker_Day_28</t>
+  </si>
+  <si>
+    <t>1
+2
+3
+4
+5
+6
+7
+8
+9
+10
+11
+12
+13
+14
+15
+16
+17
+18
+19
+20
+21
+22
+23
+24
+25
+26
+27
+28</t>
+    <phoneticPr fontId="8" type="noConversion"/>
   </si>
   <si>
     <t>Datepicker_Day_29</t>
@@ -737,45 +773,60 @@
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
   <si>
+    <t>Percentage_Bar_readout</t>
+  </si>
+  <si>
+    <t>PercentageBarReadout</t>
+  </si>
+  <si>
+    <t>&lt;value&gt;%</t>
+  </si>
+  <si>
+    <t>Percentage_Bar_headline</t>
+  </si>
+  <si>
+    <t>PercentageBarHeadline</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>0-9</t>
+  </si>
+  <si>
+    <t>BackLight  Level</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
     <t>time_picker_duration</t>
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
   <si>
     <t>Sleepduration</t>
+    <phoneticPr fontId="8" type="noConversion"/>
   </si>
   <si>
     <t>Sleepduration</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>1
-2
-3
-4
-5
-6
-7
-8
-9
-10
-11
-12
-13
-14
-15
-16
-17
-18
-19
-20
-21
-22
-23
-24
-25
-26
-27
-28</t>
+  </si>
+  <si>
+    <t>SleepWheel_headline</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>SleepWheel_readout</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>LEFT</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>of inactivity</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sleep
+after</t>
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
   <si>
@@ -784,8 +835,45 @@
 1 min
 2 min
 5 min
-15 min
+10 min
 30 min</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>passwordEdit</t>
+  </si>
+  <si>
+    <t>passwordheadline</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>ConnectHeadline</t>
+  </si>
+  <si>
+    <t>ButtonFont</t>
+  </si>
+  <si>
+    <t>OK</t>
+  </si>
+  <si>
+    <t>CANCLE</t>
+  </si>
+  <si>
+    <t>passwordHeadline</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>ButtonFont</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>buttonOK</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>buttonCancle</t>
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
 </sst>
@@ -1144,7 +1232,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1187,11 +1275,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="82">
@@ -1554,7 +1645,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table7" displayName="Table7" ref="B3:I100" totalsRowShown="0" tableBorderDxfId="10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table7" displayName="Table7" ref="B3:I97" totalsRowShown="0" tableBorderDxfId="10">
   <sortState ref="B4:E6">
     <sortCondition descending="1" ref="B3:B65536"/>
   </sortState>
@@ -1586,7 +1677,7 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Table8" displayName="Table8" ref="B3:I796" totalsRowShown="0" tableBorderDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Table8" displayName="Table8" ref="B3:I795" totalsRowShown="0" tableBorderDxfId="0">
   <tableColumns count="8">
     <tableColumn id="1" name="Text ID"/>
     <tableColumn id="2" name="Typography Name"/>
@@ -1973,29 +2064,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:O23"/>
+  <dimension ref="B1:O27"/>
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="0.33203125" customWidth="1"/>
-    <col min="2" max="2" width="25.6640625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="26.88671875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="10.44140625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="0.28515625" customWidth="1"/>
+    <col min="2" max="2" width="25.7109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="26.85546875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="10.42578125" style="1" customWidth="1"/>
     <col min="5" max="5" width="10" style="1" customWidth="1"/>
-    <col min="6" max="6" width="19.5546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="51.109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.109375" customWidth="1"/>
-    <col min="10" max="10" width="4.5546875" customWidth="1"/>
-    <col min="11" max="11" width="20.109375" customWidth="1"/>
-    <col min="12" max="12" width="84.6640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="51.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.140625" customWidth="1"/>
+    <col min="10" max="10" width="4.5703125" customWidth="1"/>
+    <col min="11" max="11" width="20.140625" customWidth="1"/>
+    <col min="12" max="12" width="84.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="11" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="19.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:15" ht="129" hidden="1" customHeight="1">
@@ -2004,19 +2095,19 @@
       <c r="D1"/>
       <c r="E1"/>
     </row>
-    <row r="2" spans="2:15" ht="39.9" customHeight="1" thickBot="1">
-      <c r="B2" s="28" t="s">
+    <row r="2" spans="2:15" ht="39.950000000000003" customHeight="1" thickBot="1">
+      <c r="B2" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="28"/>
-      <c r="D2" s="28"/>
-      <c r="E2" s="28"/>
-      <c r="F2" s="28"/>
-      <c r="G2" s="28"/>
-      <c r="H2" s="28"/>
+      <c r="C2" s="30"/>
+      <c r="D2" s="30"/>
+      <c r="E2" s="30"/>
+      <c r="F2" s="30"/>
+      <c r="G2" s="30"/>
+      <c r="H2" s="30"/>
       <c r="I2" s="3"/>
     </row>
-    <row r="3" spans="2:15" ht="15" thickBot="1">
+    <row r="3" spans="2:15" ht="15.75" thickBot="1">
       <c r="B3" s="17" t="s">
         <v>8</v>
       </c>
@@ -2044,7 +2135,7 @@
     </row>
     <row r="4" spans="2:15">
       <c r="B4" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="C4" t="s">
         <v>40</v>
@@ -2053,7 +2144,7 @@
         <v>16</v>
       </c>
       <c r="E4">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="K4" s="4" t="s">
         <v>17</v>
@@ -2082,7 +2173,7 @@
         <v>40</v>
       </c>
       <c r="E5">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="K5" s="7" t="s">
         <v>1</v>
@@ -2100,7 +2191,7 @@
     </row>
     <row r="6" spans="2:15">
       <c r="B6" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C6" t="s">
         <v>40</v>
@@ -2109,7 +2200,7 @@
         <v>12</v>
       </c>
       <c r="E6">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="K6" s="7" t="s">
         <v>2</v>
@@ -2129,20 +2220,20 @@
       <c r="B7" t="s">
         <v>57</v>
       </c>
-      <c r="C7" t="s">
-        <v>40</v>
+      <c r="C7" s="24" t="s">
+        <v>177</v>
       </c>
       <c r="D7">
         <v>16</v>
       </c>
       <c r="E7">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G7" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="H7" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="K7" s="7" t="s">
         <v>15</v>
@@ -2171,7 +2262,7 @@
         <v>16</v>
       </c>
       <c r="E8">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="K8" s="7" t="s">
         <v>16</v>
@@ -2198,7 +2289,7 @@
         <v>18</v>
       </c>
       <c r="E9">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="K9" s="11" t="s">
         <v>14</v>
@@ -2227,7 +2318,7 @@
         <v>16</v>
       </c>
       <c r="E10">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="K10" s="11" t="s">
         <v>36</v>
@@ -2245,7 +2336,7 @@
     </row>
     <row r="11" spans="2:15">
       <c r="B11" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C11" t="s">
         <v>40</v>
@@ -2254,19 +2345,19 @@
         <v>20</v>
       </c>
       <c r="E11">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G11" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="H11" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="K11" s="15"/>
     </row>
     <row r="12" spans="2:15">
       <c r="B12" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C12" t="s">
         <v>40</v>
@@ -2275,13 +2366,13 @@
         <v>20</v>
       </c>
       <c r="E12">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G12" t="s">
+        <v>101</v>
+      </c>
+      <c r="H12" t="s">
         <v>100</v>
-      </c>
-      <c r="H12" t="s">
-        <v>99</v>
       </c>
       <c r="L12" s="16" t="s">
         <v>35</v>
@@ -2289,7 +2380,7 @@
     </row>
     <row r="13" spans="2:15">
       <c r="B13" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="C13" t="s">
         <v>40</v>
@@ -2298,26 +2389,26 @@
         <v>16</v>
       </c>
       <c r="E13">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="14" spans="2:15">
       <c r="B14" t="s">
+        <v>155</v>
+      </c>
+      <c r="C14" t="s">
         <v>154</v>
-      </c>
-      <c r="C14" t="s">
-        <v>153</v>
       </c>
       <c r="D14">
         <v>75</v>
       </c>
       <c r="E14">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="15" spans="2:15">
       <c r="B15" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C15" t="s">
         <v>40</v>
@@ -2326,15 +2417,15 @@
         <v>60</v>
       </c>
       <c r="E15">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H15" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
     <row r="16" spans="2:15">
       <c r="B16" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="C16" t="s">
         <v>40</v>
@@ -2343,18 +2434,18 @@
         <v>20</v>
       </c>
       <c r="E16">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F16" t="s">
         <v>25</v>
       </c>
       <c r="G16" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
     </row>
     <row r="17" spans="2:8">
       <c r="B17" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="C17" t="s">
         <v>40</v>
@@ -2363,12 +2454,12 @@
         <v>18</v>
       </c>
       <c r="E17">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="18" spans="2:8">
       <c r="B18" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="C18" t="s">
         <v>40</v>
@@ -2377,12 +2468,12 @@
         <v>18</v>
       </c>
       <c r="E18">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="19" spans="2:8">
       <c r="B19" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="C19" t="s">
         <v>40</v>
@@ -2391,7 +2482,7 @@
         <v>16</v>
       </c>
       <c r="E19">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F19" t="s">
         <v>25</v>
@@ -2399,10 +2490,10 @@
     </row>
     <row r="20" spans="2:8">
       <c r="B20" s="22" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="C20" s="24" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="D20" s="22">
         <v>28</v>
@@ -2414,18 +2505,18 @@
         <v>25</v>
       </c>
       <c r="G20" s="25" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="H20" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
     <row r="21" spans="2:8">
       <c r="B21" s="22" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="C21" s="24" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="D21" s="22">
         <v>20</v>
@@ -2437,18 +2528,18 @@
         <v>25</v>
       </c>
       <c r="G21" s="26" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="H21" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
     <row r="22" spans="2:8">
       <c r="B22" s="22" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="C22" s="24" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="D22" s="22">
         <v>24</v>
@@ -2459,15 +2550,77 @@
     </row>
     <row r="23" spans="2:8">
       <c r="B23" s="1" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C23" s="24" t="s">
-        <v>176</v>
-      </c>
-      <c r="D23" s="22">
+        <v>177</v>
+      </c>
+      <c r="D23" s="1">
         <v>16</v>
       </c>
-      <c r="E23" s="22">
+      <c r="E23" s="1">
+        <v>4</v>
+      </c>
+      <c r="G23" s="28" t="s">
+        <v>186</v>
+      </c>
+      <c r="H23" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="24" spans="2:8">
+      <c r="B24" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="C24" s="24" t="s">
+        <v>177</v>
+      </c>
+      <c r="D24" s="1">
+        <v>16</v>
+      </c>
+      <c r="E24" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="25" spans="2:8">
+      <c r="B25" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="C25" s="24" t="s">
+        <v>177</v>
+      </c>
+      <c r="D25" s="22">
+        <v>16</v>
+      </c>
+      <c r="E25" s="22">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="26" spans="2:8">
+      <c r="B26" t="s">
+        <v>199</v>
+      </c>
+      <c r="C26" t="s">
+        <v>40</v>
+      </c>
+      <c r="D26">
+        <v>14</v>
+      </c>
+      <c r="E26">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="27" spans="2:8">
+      <c r="B27" t="s">
+        <v>202</v>
+      </c>
+      <c r="C27" t="s">
+        <v>40</v>
+      </c>
+      <c r="D27">
+        <v>12</v>
+      </c>
+      <c r="E27">
         <v>4</v>
       </c>
     </row>
@@ -2489,21 +2642,21 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:J64"/>
+  <dimension ref="B1:J73"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A56" workbookViewId="0">
-      <selection activeCell="E64" sqref="E64"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A65" workbookViewId="0">
+      <selection activeCell="B73" sqref="B73"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="0.33203125" customWidth="1"/>
-    <col min="2" max="2" width="54.6640625" style="1" customWidth="1"/>
-    <col min="3" max="4" width="25.6640625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="35.6640625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="50.6640625" style="1" customWidth="1"/>
-    <col min="7" max="8" width="8.6640625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="54.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="0.28515625" customWidth="1"/>
+    <col min="2" max="2" width="54.7109375" style="1" customWidth="1"/>
+    <col min="3" max="4" width="25.7109375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="35.7109375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="50.7109375" style="1" customWidth="1"/>
+    <col min="7" max="8" width="8.7109375" style="1" customWidth="1"/>
+    <col min="9" max="9" width="54.28515625" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:10" ht="129" hidden="1" customHeight="1">
@@ -2516,17 +2669,17 @@
       <c r="H1"/>
       <c r="I1"/>
     </row>
-    <row r="2" spans="2:10" ht="39.9" customHeight="1">
-      <c r="B2" s="28" t="s">
+    <row r="2" spans="2:10" ht="39.950000000000003" customHeight="1">
+      <c r="B2" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="28"/>
-      <c r="D2" s="28"/>
-      <c r="E2" s="28"/>
-      <c r="F2" s="28"/>
-      <c r="G2" s="28"/>
-      <c r="H2" s="28"/>
-      <c r="I2" s="28"/>
+      <c r="C2" s="30"/>
+      <c r="D2" s="30"/>
+      <c r="E2" s="30"/>
+      <c r="F2" s="30"/>
+      <c r="G2" s="30"/>
+      <c r="H2" s="30"/>
+      <c r="I2" s="30"/>
       <c r="J2" t="s">
         <v>13</v>
       </c>
@@ -2565,7 +2718,7 @@
         <v>57</v>
       </c>
       <c r="D4" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="E4" t="s">
         <v>43</v>
@@ -2739,7 +2892,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="17" spans="2:5">
+    <row r="17" spans="2:5" ht="345">
       <c r="B17" t="s">
         <v>67</v>
       </c>
@@ -2749,11 +2902,11 @@
       <c r="D17" t="s">
         <v>42</v>
       </c>
-      <c r="E17" t="s">
+      <c r="E17" s="29" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="18" spans="2:5">
+    <row r="18" spans="2:5" ht="375">
       <c r="B18" t="s">
         <v>70</v>
       </c>
@@ -2763,11 +2916,11 @@
       <c r="D18" t="s">
         <v>42</v>
       </c>
-      <c r="E18" t="s">
+      <c r="E18" s="29" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="19" spans="2:5" ht="409.6">
+    <row r="19" spans="2:5">
       <c r="B19" t="s">
         <v>72</v>
       </c>
@@ -2777,13 +2930,13 @@
       <c r="D19" t="s">
         <v>42</v>
       </c>
-      <c r="E19" s="29" t="s">
-        <v>183</v>
+      <c r="E19" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="20" spans="2:5">
       <c r="B20" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C20" t="s">
         <v>68</v>
@@ -2792,12 +2945,12 @@
         <v>42</v>
       </c>
       <c r="E20" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="21" spans="2:5">
       <c r="B21" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C21" t="s">
         <v>68</v>
@@ -2806,12 +2959,12 @@
         <v>42</v>
       </c>
       <c r="E21" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="22" spans="2:5">
       <c r="B22" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C22" t="s">
         <v>68</v>
@@ -2820,43 +2973,43 @@
         <v>42</v>
       </c>
       <c r="E22" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="23" spans="2:5">
       <c r="B23" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C23" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="D23" t="s">
         <v>42</v>
       </c>
       <c r="E23" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="24" spans="2:5">
       <c r="B24" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C24" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="D24" t="s">
         <v>42</v>
       </c>
       <c r="E24" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="25" spans="2:5">
       <c r="B25" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C25" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="D25" t="s">
         <v>66</v>
@@ -2867,21 +3020,21 @@
     </row>
     <row r="26" spans="2:5">
       <c r="B26" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C26" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="D26" t="s">
         <v>42</v>
       </c>
       <c r="E26" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="27" spans="2:5">
       <c r="B27" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C27" t="s">
         <v>57</v>
@@ -2895,24 +3048,24 @@
     </row>
     <row r="28" spans="2:5">
       <c r="B28" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C28" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="D28" t="s">
         <v>42</v>
       </c>
       <c r="E28" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
     <row r="29" spans="2:5">
       <c r="B29" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C29" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="D29" t="s">
         <v>66</v>
@@ -2923,276 +3076,276 @@
     </row>
     <row r="30" spans="2:5">
       <c r="B30" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C30" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="D30" t="s">
         <v>42</v>
       </c>
       <c r="E30" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="31" spans="2:5">
       <c r="B31" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C31" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="D31" t="s">
         <v>42</v>
       </c>
       <c r="E31" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
     <row r="32" spans="2:5">
       <c r="B32" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C32" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="D32" t="s">
         <v>42</v>
       </c>
       <c r="E32" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="33" spans="2:5">
       <c r="B33" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C33" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="D33" t="s">
         <v>42</v>
       </c>
       <c r="E33" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="34" spans="2:5">
       <c r="B34" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C34" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="D34" t="s">
         <v>42</v>
       </c>
       <c r="E34" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="35" spans="2:5">
       <c r="B35" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C35" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="D35" t="s">
         <v>42</v>
       </c>
       <c r="E35" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
     </row>
     <row r="36" spans="2:5">
       <c r="B36" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C36" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="D36" t="s">
         <v>42</v>
       </c>
       <c r="E36" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="37" spans="2:5">
       <c r="B37" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C37" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="D37" t="s">
         <v>42</v>
       </c>
       <c r="E37" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
     </row>
     <row r="38" spans="2:5">
       <c r="B38" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C38" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="D38" t="s">
         <v>42</v>
       </c>
       <c r="E38" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
     </row>
     <row r="39" spans="2:5">
       <c r="B39" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C39" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="D39" t="s">
         <v>42</v>
       </c>
       <c r="E39" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="40" spans="2:5">
       <c r="B40" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C40" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="D40" t="s">
         <v>42</v>
       </c>
       <c r="E40" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
     </row>
     <row r="41" spans="2:5">
       <c r="B41" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="C41" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="D41" t="s">
         <v>42</v>
       </c>
       <c r="E41" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
     </row>
     <row r="42" spans="2:5">
       <c r="B42" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C42" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="D42" t="s">
         <v>42</v>
       </c>
       <c r="E42" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
     </row>
     <row r="43" spans="2:5">
       <c r="B43" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C43" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="D43" t="s">
         <v>42</v>
       </c>
       <c r="E43" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
     </row>
     <row r="44" spans="2:5">
       <c r="B44" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C44" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="D44" t="s">
         <v>42</v>
       </c>
       <c r="E44" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
     </row>
     <row r="45" spans="2:5">
       <c r="B45" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C45" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="D45" t="s">
         <v>42</v>
       </c>
       <c r="E45" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="46" spans="2:5">
       <c r="B46" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C46" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="D46" t="s">
         <v>42</v>
       </c>
       <c r="E46" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
     </row>
     <row r="47" spans="2:5">
       <c r="B47" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="C47" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="D47" t="s">
         <v>42</v>
       </c>
       <c r="E47" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="48" spans="2:5">
       <c r="B48" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="C48" t="s">
+        <v>140</v>
+      </c>
+      <c r="D48" t="s">
+        <v>42</v>
+      </c>
+      <c r="E48" t="s">
         <v>139</v>
       </c>
-      <c r="D48" t="s">
-        <v>42</v>
-      </c>
-      <c r="E48" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="49" spans="2:5">
+    </row>
+    <row r="49" spans="2:6">
       <c r="B49" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="C49" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="D49" t="s">
         <v>42</v>
@@ -3201,12 +3354,12 @@
         <v>43</v>
       </c>
     </row>
-    <row r="50" spans="2:5">
+    <row r="50" spans="2:6">
       <c r="B50" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="C50" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="D50" t="s">
         <v>66</v>
@@ -3215,12 +3368,12 @@
         <v>43</v>
       </c>
     </row>
-    <row r="51" spans="2:5">
+    <row r="51" spans="2:6">
       <c r="B51" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C51" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="D51" t="s">
         <v>66</v>
@@ -3229,186 +3382,311 @@
         <v>43</v>
       </c>
     </row>
-    <row r="52" spans="2:5">
+    <row r="52" spans="2:6">
       <c r="B52" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="C52" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="D52" t="s">
         <v>66</v>
       </c>
       <c r="E52" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="53" spans="2:5">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="53" spans="2:6">
       <c r="B53" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="C53" t="s">
+        <v>150</v>
+      </c>
+      <c r="D53" t="s">
         <v>149</v>
       </c>
-      <c r="D53" t="s">
+      <c r="E53" t="s">
         <v>148</v>
       </c>
-      <c r="E53" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="54" spans="2:5">
+    </row>
+    <row r="54" spans="2:6">
       <c r="B54" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="C54" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="D54" t="s">
         <v>42</v>
       </c>
       <c r="E54" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="55" spans="2:5">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="55" spans="2:6">
       <c r="B55" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="C55" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D55" t="s">
         <v>42</v>
       </c>
       <c r="E55" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="56" spans="2:5">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="56" spans="2:6">
       <c r="B56" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C56" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="D56" t="s">
         <v>66</v>
       </c>
       <c r="E56" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="57" spans="2:5">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="57" spans="2:6">
       <c r="B57" t="s">
+        <v>160</v>
+      </c>
+      <c r="C57" t="s">
         <v>159</v>
       </c>
-      <c r="C57" t="s">
+      <c r="D57" t="s">
+        <v>42</v>
+      </c>
+      <c r="E57" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="58" spans="2:6">
+      <c r="B58" t="s">
         <v>158</v>
       </c>
-      <c r="D57" t="s">
-        <v>42</v>
-      </c>
-      <c r="E57" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="58" spans="2:5">
-      <c r="B58" t="s">
-        <v>157</v>
-      </c>
       <c r="C58" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="D58" t="s">
         <v>42</v>
       </c>
       <c r="E58" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="59" spans="2:5">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="59" spans="2:6">
       <c r="B59" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="C59" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="D59" t="s">
         <v>66</v>
       </c>
       <c r="E59" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="60" spans="2:5">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="60" spans="2:6">
       <c r="B60" s="1" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="C60" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D60" t="s">
         <v>66</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="61" spans="2:5">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="61" spans="2:6">
       <c r="B61" s="22" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="C61" s="22" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="D61" s="22" t="s">
         <v>42</v>
       </c>
       <c r="E61" s="23" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="62" spans="2:5">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="62" spans="2:6">
       <c r="B62" s="22" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="C62" s="22" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="D62" s="22" t="s">
         <v>66</v>
       </c>
       <c r="E62" s="23" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="63" spans="2:6">
+      <c r="B63" s="22" t="s">
+        <v>175</v>
+      </c>
+      <c r="C63" s="22" t="s">
         <v>173</v>
-      </c>
-    </row>
-    <row r="63" spans="2:5">
-      <c r="B63" s="22" t="s">
-        <v>174</v>
-      </c>
-      <c r="C63" s="22" t="s">
-        <v>172</v>
       </c>
       <c r="D63" s="22" t="s">
         <v>66</v>
       </c>
       <c r="E63" s="23" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="64" spans="2:5" ht="187.2">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="64" spans="2:6">
       <c r="B64" s="1" t="s">
-        <v>180</v>
-      </c>
-      <c r="C64" t="s">
+        <v>181</v>
+      </c>
+      <c r="C64" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="D64" s="22" t="s">
-        <v>42</v>
+      <c r="D64" t="s">
+        <v>66</v>
       </c>
       <c r="E64" s="27" t="s">
+        <v>183</v>
+      </c>
+      <c r="F64" s="27"/>
+    </row>
+    <row r="65" spans="2:6">
+      <c r="B65" s="1" t="s">
         <v>184</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="E65" s="27" t="s">
+        <v>188</v>
+      </c>
+      <c r="F65" s="28"/>
+    </row>
+    <row r="66" spans="2:6">
+      <c r="B66" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="C66" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="D66" t="s">
+        <v>66</v>
+      </c>
+      <c r="E66" s="27" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="67" spans="2:6" ht="30">
+      <c r="B67" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="C67" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="D67" s="22" t="s">
+        <v>194</v>
+      </c>
+      <c r="E67" s="27" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="68" spans="2:6" ht="195">
+      <c r="B68" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="C68" t="s">
+        <v>190</v>
+      </c>
+      <c r="D68" s="22" t="s">
+        <v>42</v>
+      </c>
+      <c r="E68" s="29" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="69" spans="2:6">
+      <c r="B69" t="s">
+        <v>198</v>
+      </c>
+      <c r="C69" t="s">
+        <v>151</v>
+      </c>
+      <c r="D69" t="s">
+        <v>42</v>
+      </c>
+      <c r="E69" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="70" spans="2:6">
+      <c r="B70" t="s">
+        <v>205</v>
+      </c>
+      <c r="C70" t="s">
+        <v>199</v>
+      </c>
+      <c r="D70" t="s">
+        <v>42</v>
+      </c>
+      <c r="E70" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="71" spans="2:6">
+      <c r="B71" t="s">
+        <v>201</v>
+      </c>
+      <c r="C71" t="s">
+        <v>151</v>
+      </c>
+      <c r="D71" t="s">
+        <v>42</v>
+      </c>
+      <c r="E71" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="72" spans="2:6">
+      <c r="B72" t="s">
+        <v>207</v>
+      </c>
+      <c r="C72" t="s">
+        <v>202</v>
+      </c>
+      <c r="D72" t="s">
+        <v>66</v>
+      </c>
+      <c r="E72" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="73" spans="2:6">
+      <c r="B73" t="s">
+        <v>208</v>
+      </c>
+      <c r="C73" t="s">
+        <v>206</v>
+      </c>
+      <c r="D73" t="s">
+        <v>66</v>
+      </c>
+      <c r="E73" t="s">
+        <v>204</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
console simulator & input screen
</commit_message>
<xml_diff>
--- a/touchGFX/Application/assets/texts/texts.xlsx
+++ b/touchGFX/Application/assets/texts/texts.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8196"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8196" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Typography" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="404" uniqueCount="218">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="408" uniqueCount="223">
   <si>
     <t>Font</t>
   </si>
@@ -801,104 +801,125 @@
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
   <si>
+    <t>passwordheadline</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>ConnectHeadline</t>
+  </si>
+  <si>
+    <t>ButtonFont</t>
+  </si>
+  <si>
+    <t>OK</t>
+  </si>
+  <si>
+    <t>CANCLE</t>
+  </si>
+  <si>
+    <t>passwordHeadline</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>ButtonFont</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>buttonOK</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>buttonCancle</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>startRecord</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>Hold to Talk</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>endRecord</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>Release to Send</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>CancelRecord</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>Slide up to Cancel</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>releaseCancel</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>Release to Cancel</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>verdana.ttf</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;value&gt;</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>15sec     30sec      1min      2min      5min     10min     30min</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>verdana.ttf</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>lucon.TTF</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sleepduration</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>time_picker_duration</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>PercentageBarReadout</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>LEFT</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
     <t>passwordEdit</t>
-  </si>
-  <si>
-    <t>passwordheadline</t>
-  </si>
-  <si>
-    <t>Password</t>
-  </si>
-  <si>
-    <t>ConnectHeadline</t>
-  </si>
-  <si>
-    <t>ButtonFont</t>
-  </si>
-  <si>
-    <t>OK</t>
-  </si>
-  <si>
-    <t>CANCLE</t>
-  </si>
-  <si>
-    <t>passwordHeadline</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>ButtonFont</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>buttonOK</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>buttonCancle</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>startRecord</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>Hold to Talk</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>endRecord</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>Release to Send</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>CancelRecord</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>Slide up to Cancel</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>releaseCancel</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>Release to Cancel</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>verdana.ttf</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>&lt;value&gt;</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>Sleep after &lt;value&gt; of inactivity</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>15sec     30sec      1min      2min      5min     10min     30min</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>verdana.ttf</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>lucon.TTF</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>Sleepduration</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>time_picker_duration</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sleep</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>after &lt;value&gt; of inactivity</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>SleepWheel_headline</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>Display</t>
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
 </sst>
@@ -1702,7 +1723,7 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Table8" displayName="Table8" ref="B3:I794" totalsRowShown="0" tableBorderDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Table8" displayName="Table8" ref="B3:I795" totalsRowShown="0" tableBorderDxfId="0">
   <tableColumns count="8">
     <tableColumn id="1" name="Text ID"/>
     <tableColumn id="2" name="Typography Name"/>
@@ -2091,8 +2112,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:O27"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView showGridLines="0" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -2515,13 +2536,13 @@
     </row>
     <row r="20" spans="2:8">
       <c r="B20" s="22" t="s">
-        <v>170</v>
+        <v>222</v>
       </c>
       <c r="C20" s="24" t="s">
         <v>177</v>
       </c>
       <c r="D20" s="22">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="E20" s="22">
         <v>4</v>
@@ -2598,7 +2619,7 @@
         <v>185</v>
       </c>
       <c r="C24" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="D24" s="1">
         <v>16</v>
@@ -2609,10 +2630,10 @@
     </row>
     <row r="25" spans="2:8">
       <c r="B25" s="1" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C25" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="D25" s="22">
         <v>12</v>
@@ -2623,10 +2644,10 @@
     </row>
     <row r="26" spans="2:8">
       <c r="B26" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C26" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D26">
         <v>14</v>
@@ -2637,7 +2658,7 @@
     </row>
     <row r="27" spans="2:8">
       <c r="B27" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C27" t="s">
         <v>40</v>
@@ -2667,10 +2688,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:J76"/>
+  <dimension ref="B1:J77"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A50" workbookViewId="0">
-      <selection activeCell="B66" sqref="B66"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A50" workbookViewId="0">
+      <selection activeCell="B61" sqref="B61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -3580,7 +3601,7 @@
         <v>181</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>182</v>
+        <v>216</v>
       </c>
       <c r="D64" t="s">
         <v>66</v>
@@ -3604,7 +3625,7 @@
     </row>
     <row r="66" spans="2:6">
       <c r="B66" s="1" t="s">
-        <v>190</v>
+        <v>221</v>
       </c>
       <c r="C66" s="1" t="s">
         <v>185</v>
@@ -3613,147 +3634,161 @@
         <v>66</v>
       </c>
       <c r="E66" s="27" t="s">
-        <v>212</v>
+        <v>219</v>
       </c>
     </row>
     <row r="67" spans="2:6">
       <c r="B67" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="C67" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="D67" t="s">
+        <v>66</v>
+      </c>
+      <c r="E67" s="27" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="68" spans="2:6">
+      <c r="B68" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="C68" t="s">
+        <v>189</v>
+      </c>
+      <c r="D68" s="22" t="s">
         <v>217</v>
       </c>
-      <c r="C67" t="s">
-        <v>189</v>
-      </c>
-      <c r="D67" s="22" t="s">
-        <v>42</v>
-      </c>
-      <c r="E67" s="29" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="68" spans="2:6">
-      <c r="B68" t="s">
-        <v>191</v>
-      </c>
-      <c r="C68" t="s">
-        <v>151</v>
-      </c>
-      <c r="D68" t="s">
-        <v>42</v>
-      </c>
-      <c r="E68" t="s">
-        <v>43</v>
+      <c r="E68" s="29" t="s">
+        <v>211</v>
       </c>
     </row>
     <row r="69" spans="2:6">
       <c r="B69" t="s">
-        <v>198</v>
+        <v>218</v>
       </c>
       <c r="C69" t="s">
-        <v>192</v>
+        <v>151</v>
       </c>
       <c r="D69" t="s">
         <v>42</v>
       </c>
       <c r="E69" t="s">
-        <v>193</v>
+        <v>43</v>
       </c>
     </row>
     <row r="70" spans="2:6">
       <c r="B70" t="s">
-        <v>194</v>
+        <v>197</v>
       </c>
       <c r="C70" t="s">
-        <v>151</v>
+        <v>191</v>
       </c>
       <c r="D70" t="s">
         <v>42</v>
       </c>
       <c r="E70" t="s">
-        <v>211</v>
+        <v>192</v>
       </c>
     </row>
     <row r="71" spans="2:6">
       <c r="B71" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="C71" t="s">
-        <v>195</v>
+        <v>151</v>
       </c>
       <c r="D71" t="s">
-        <v>66</v>
+        <v>42</v>
       </c>
       <c r="E71" t="s">
-        <v>196</v>
+        <v>210</v>
       </c>
     </row>
     <row r="72" spans="2:6">
       <c r="B72" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="C72" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="D72" t="s">
         <v>66</v>
       </c>
       <c r="E72" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="73" spans="2:6">
       <c r="B73" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C73" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="D73" t="s">
         <v>66</v>
       </c>
       <c r="E73" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
     </row>
     <row r="74" spans="2:6">
       <c r="B74" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="C74" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D74" t="s">
         <v>66</v>
       </c>
       <c r="E74" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
     </row>
     <row r="75" spans="2:6">
       <c r="B75" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="C75" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D75" t="s">
         <v>66</v>
       </c>
       <c r="E75" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
     </row>
     <row r="76" spans="2:6">
-      <c r="B76" s="1" t="s">
-        <v>208</v>
+      <c r="B76" t="s">
+        <v>205</v>
       </c>
       <c r="C76" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D76" t="s">
         <v>66</v>
       </c>
-      <c r="E76" s="1" t="s">
-        <v>209</v>
+      <c r="E76" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="77" spans="2:6">
+      <c r="B77" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="C77" t="s">
+        <v>194</v>
+      </c>
+      <c r="D77" t="s">
+        <v>66</v>
+      </c>
+      <c r="E77" s="1" t="s">
+        <v>208</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add in the clock screen to show date
</commit_message>
<xml_diff>
--- a/touchGFX/Application/assets/texts/texts.xlsx
+++ b/touchGFX/Application/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="408" uniqueCount="223">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="412" uniqueCount="225">
   <si>
     <t>Font</t>
   </si>
@@ -807,115 +807,124 @@
     <t>Password</t>
   </si>
   <si>
+    <t>ButtonFont</t>
+  </si>
+  <si>
+    <t>OK</t>
+  </si>
+  <si>
+    <t>CANCLE</t>
+  </si>
+  <si>
+    <t>passwordHeadline</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>ButtonFont</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>buttonOK</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>buttonCancle</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>startRecord</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>Hold to Talk</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>endRecord</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>Release to Send</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>CancelRecord</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>Slide up to Cancel</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>releaseCancel</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>Release to Cancel</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>verdana.ttf</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;value&gt;</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>15sec     30sec      1min      2min      5min     10min     30min</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>verdana.ttf</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>lucon.TTF</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sleepduration</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>time_picker_duration</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>PercentageBarReadout</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>LEFT</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>passwordEdit</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sleep</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>after &lt;value&gt; of inactivity</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>SleepWheel_headline</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;value&gt;</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
     <t>ConnectHeadline</t>
-  </si>
-  <si>
-    <t>ButtonFont</t>
-  </si>
-  <si>
-    <t>OK</t>
-  </si>
-  <si>
-    <t>CANCLE</t>
-  </si>
-  <si>
-    <t>passwordHeadline</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>ButtonFont</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>buttonOK</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>buttonCancle</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>startRecord</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>Hold to Talk</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>endRecord</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>Release to Send</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>CancelRecord</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>Slide up to Cancel</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>releaseCancel</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>Release to Cancel</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>verdana.ttf</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>&lt;value&gt;</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>15sec     30sec      1min      2min      5min     10min     30min</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>verdana.ttf</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>lucon.TTF</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>Sleepduration</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>time_picker_duration</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>PercentageBarReadout</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>LEFT</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>passwordEdit</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>Sleep</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>after &lt;value&gt; of inactivity</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>SleepWheel_headline</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>dateText</t>
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
   <si>
@@ -2113,7 +2122,7 @@
   <dimension ref="B1:O27"/>
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -2536,7 +2545,7 @@
     </row>
     <row r="20" spans="2:8">
       <c r="B20" s="22" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="C20" s="24" t="s">
         <v>177</v>
@@ -2619,7 +2628,7 @@
         <v>185</v>
       </c>
       <c r="C24" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D24" s="1">
         <v>16</v>
@@ -2630,10 +2639,10 @@
     </row>
     <row r="25" spans="2:8">
       <c r="B25" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C25" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D25" s="22">
         <v>12</v>
@@ -2647,7 +2656,7 @@
         <v>191</v>
       </c>
       <c r="C26" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D26">
         <v>14</v>
@@ -2658,7 +2667,7 @@
     </row>
     <row r="27" spans="2:8">
       <c r="B27" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C27" t="s">
         <v>40</v>
@@ -2688,10 +2697,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:J77"/>
+  <dimension ref="B1:J78"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A50" workbookViewId="0">
-      <selection activeCell="B61" sqref="B61"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -3125,7 +3134,7 @@
         <v>102</v>
       </c>
       <c r="C30" t="s">
-        <v>140</v>
+        <v>151</v>
       </c>
       <c r="D30" t="s">
         <v>42</v>
@@ -3139,7 +3148,7 @@
         <v>104</v>
       </c>
       <c r="C31" t="s">
-        <v>140</v>
+        <v>151</v>
       </c>
       <c r="D31" t="s">
         <v>42</v>
@@ -3153,7 +3162,7 @@
         <v>106</v>
       </c>
       <c r="C32" t="s">
-        <v>140</v>
+        <v>151</v>
       </c>
       <c r="D32" t="s">
         <v>42</v>
@@ -3167,7 +3176,7 @@
         <v>108</v>
       </c>
       <c r="C33" t="s">
-        <v>140</v>
+        <v>151</v>
       </c>
       <c r="D33" t="s">
         <v>42</v>
@@ -3181,7 +3190,7 @@
         <v>110</v>
       </c>
       <c r="C34" t="s">
-        <v>140</v>
+        <v>151</v>
       </c>
       <c r="D34" t="s">
         <v>42</v>
@@ -3195,7 +3204,7 @@
         <v>112</v>
       </c>
       <c r="C35" t="s">
-        <v>140</v>
+        <v>151</v>
       </c>
       <c r="D35" t="s">
         <v>42</v>
@@ -3209,7 +3218,7 @@
         <v>114</v>
       </c>
       <c r="C36" t="s">
-        <v>140</v>
+        <v>151</v>
       </c>
       <c r="D36" t="s">
         <v>42</v>
@@ -3601,7 +3610,7 @@
         <v>181</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D64" t="s">
         <v>66</v>
@@ -3625,7 +3634,7 @@
     </row>
     <row r="66" spans="2:6">
       <c r="B66" s="1" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C66" s="1" t="s">
         <v>185</v>
@@ -3634,7 +3643,7 @@
         <v>66</v>
       </c>
       <c r="E66" s="27" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="67" spans="2:6">
@@ -3648,26 +3657,26 @@
         <v>66</v>
       </c>
       <c r="E67" s="27" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="68" spans="2:6">
       <c r="B68" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C68" t="s">
         <v>189</v>
       </c>
       <c r="D68" s="22" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E68" s="29" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="69" spans="2:6">
       <c r="B69" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C69" t="s">
         <v>151</v>
@@ -3681,7 +3690,7 @@
     </row>
     <row r="70" spans="2:6">
       <c r="B70" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C70" t="s">
         <v>191</v>
@@ -3695,7 +3704,7 @@
     </row>
     <row r="71" spans="2:6">
       <c r="B71" t="s">
-        <v>193</v>
+        <v>222</v>
       </c>
       <c r="C71" t="s">
         <v>151</v>
@@ -3704,91 +3713,105 @@
         <v>42</v>
       </c>
       <c r="E71" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="72" spans="2:6">
       <c r="B72" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C72" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D72" t="s">
         <v>66</v>
       </c>
       <c r="E72" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="73" spans="2:6">
       <c r="B73" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C73" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D73" t="s">
         <v>66</v>
       </c>
       <c r="E73" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="74" spans="2:6">
       <c r="B74" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C74" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D74" t="s">
         <v>66</v>
       </c>
       <c r="E74" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="75" spans="2:6">
       <c r="B75" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C75" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D75" t="s">
         <v>66</v>
       </c>
       <c r="E75" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="76" spans="2:6">
       <c r="B76" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C76" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D76" t="s">
         <v>66</v>
       </c>
       <c r="E76" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="77" spans="2:6">
       <c r="B77" s="1" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C77" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D77" t="s">
         <v>66</v>
       </c>
       <c r="E77" s="1" t="s">
-        <v>208</v>
+        <v>207</v>
+      </c>
+    </row>
+    <row r="78" spans="2:6">
+      <c r="B78" t="s">
+        <v>223</v>
+      </c>
+      <c r="C78" t="s">
+        <v>151</v>
+      </c>
+      <c r="D78" t="s">
+        <v>66</v>
+      </c>
+      <c r="E78" t="s">
+        <v>221</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix mainmenu and mic view
</commit_message>
<xml_diff>
--- a/touchGFX/Application/assets/texts/texts.xlsx
+++ b/touchGFX/Application/assets/texts/texts.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\L2200_TouchGFX\L2200_Remoter_changer\L2200_Remoter\touchGFX\Application\assets\texts\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8196" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Typography" sheetId="1" r:id="rId1"/>
@@ -20,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="466" uniqueCount="256">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="474" uniqueCount="260">
   <si>
     <t>Font</t>
   </si>
@@ -1053,6 +1048,22 @@
   </si>
   <si>
     <t>.-+</t>
+  </si>
+  <si>
+    <t>Sending</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>MicSendingTxt</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>Finish</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>MicSendFinishTxt</t>
+    <phoneticPr fontId="8" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -2244,27 +2255,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:O29"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29:H29"/>
+    <sheetView showGridLines="0" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="0.28515625" customWidth="1"/>
-    <col min="2" max="2" width="25.7109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="26.85546875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="10.42578125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="0.33203125" customWidth="1"/>
+    <col min="2" max="2" width="25.6640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="26.88671875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="10.44140625" style="1" customWidth="1"/>
     <col min="5" max="5" width="10" style="1" customWidth="1"/>
-    <col min="6" max="6" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="51.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.140625" customWidth="1"/>
-    <col min="10" max="10" width="4.5703125" customWidth="1"/>
-    <col min="11" max="11" width="20.140625" customWidth="1"/>
-    <col min="12" max="12" width="84.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="51.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.109375" customWidth="1"/>
+    <col min="10" max="10" width="4.5546875" customWidth="1"/>
+    <col min="11" max="11" width="20.109375" customWidth="1"/>
+    <col min="12" max="12" width="84.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.33203125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="11" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="19.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:15" ht="129" hidden="1" customHeight="1">
@@ -2273,7 +2284,7 @@
       <c r="D1"/>
       <c r="E1"/>
     </row>
-    <row r="2" spans="2:15" ht="39.950000000000003" customHeight="1" thickBot="1">
+    <row r="2" spans="2:15" ht="39.9" customHeight="1" thickBot="1">
       <c r="B2" s="30" t="s">
         <v>5</v>
       </c>
@@ -2285,7 +2296,7 @@
       <c r="H2" s="30"/>
       <c r="I2" s="3"/>
     </row>
-    <row r="3" spans="2:15" ht="15.75" thickBot="1">
+    <row r="3" spans="2:15" ht="15" thickBot="1">
       <c r="B3" s="17" t="s">
         <v>8</v>
       </c>
@@ -2854,21 +2865,21 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:J90"/>
+  <dimension ref="B1:J92"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A71" workbookViewId="0">
-      <selection activeCell="B91" sqref="B91"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A71" workbookViewId="0">
+      <selection activeCell="B92" sqref="B92"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="0.28515625" customWidth="1"/>
-    <col min="2" max="2" width="54.7109375" style="1" customWidth="1"/>
-    <col min="3" max="4" width="25.7109375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="62.42578125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="50.7109375" style="1" customWidth="1"/>
-    <col min="7" max="8" width="8.7109375" style="1" customWidth="1"/>
-    <col min="9" max="9" width="54.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="0.33203125" customWidth="1"/>
+    <col min="2" max="2" width="54.6640625" style="1" customWidth="1"/>
+    <col min="3" max="4" width="25.6640625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="62.44140625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="50.6640625" style="1" customWidth="1"/>
+    <col min="7" max="8" width="8.6640625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="54.33203125" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:10" ht="129" hidden="1" customHeight="1">
@@ -2881,7 +2892,7 @@
       <c r="H1"/>
       <c r="I1"/>
     </row>
-    <row r="2" spans="2:10" ht="39.950000000000003" customHeight="1">
+    <row r="2" spans="2:10" ht="39.9" customHeight="1">
       <c r="B2" s="30" t="s">
         <v>7</v>
       </c>
@@ -3104,7 +3115,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="17" spans="2:5" ht="345">
+    <row r="17" spans="2:5" ht="331.2">
       <c r="B17" t="s">
         <v>66</v>
       </c>
@@ -3118,7 +3129,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="18" spans="2:5" ht="375">
+    <row r="18" spans="2:5" ht="360">
       <c r="B18" t="s">
         <v>69</v>
       </c>
@@ -4137,6 +4148,34 @@
       </c>
       <c r="E90" s="1" t="s">
         <v>254</v>
+      </c>
+    </row>
+    <row r="91" spans="2:5">
+      <c r="B91" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="C91" t="s">
+        <v>241</v>
+      </c>
+      <c r="D91" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="E91" s="1" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="92" spans="2:5">
+      <c r="B92" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="C92" t="s">
+        <v>241</v>
+      </c>
+      <c r="D92" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="E92" s="1" t="s">
+        <v>258</v>
       </c>
     </row>
   </sheetData>

</xml_diff>